<commit_message>
HashTable y Util optimizados, clases mejoradas, implementacion de herencia
</commit_message>
<xml_diff>
--- a/BatesHotel/datos.xlsx
+++ b/BatesHotel/datos.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90492B21-D5DC-426A-B162-9BD95EFD7DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -72,7 +71,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -82,6 +81,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -100,9 +100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -140,7 +140,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -212,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,11 +385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>3</v>
       </c>
       <c r="F2">
@@ -447,9 +447,6 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>9</v>
-      </c>
       <c r="E3">
         <v>0</v>
       </c>
@@ -467,9 +464,6 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>55</v>
-      </c>
       <c r="E4" s="3">
         <v>44905</v>
       </c>
@@ -499,12 +493,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08177439-E9B1-4C25-A526-CCEB68998C69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>